<commit_message>
corrected OOI bar codes between bulk load, cal data, and integration event
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI03FLMA_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_GI03FLMA_00002.xlsx
@@ -641,9 +641,6 @@
     <t>N00512</t>
   </si>
   <si>
-    <t>OL000003</t>
-  </si>
-  <si>
     <t>OL000021</t>
   </si>
   <si>
@@ -651,6 +648,9 @@
   </si>
   <si>
     <t>GI03FLMA-RIM01-00-SIOENG000</t>
+  </si>
+  <si>
+    <t>OL000004</t>
   </si>
 </sst>
 </file>
@@ -1880,7 +1880,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1998,8 +1998,8 @@
   <dimension ref="A1:R131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5741,7 +5741,7 @@
     </row>
     <row r="124" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B124" t="s">
         <v>115</v>
@@ -5753,7 +5753,7 @@
         <v>2</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F124" s="51">
         <v>12372</v>
@@ -5776,19 +5776,19 @@
     </row>
     <row r="126" spans="1:15" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B126" t="s">
+        <v>115</v>
+      </c>
+      <c r="C126" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D126" s="42">
+        <v>2</v>
+      </c>
+      <c r="E126" t="s">
         <v>144</v>
-      </c>
-      <c r="B126" t="s">
-        <v>115</v>
-      </c>
-      <c r="C126" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="D126" s="42">
-        <v>2</v>
-      </c>
-      <c r="E126" t="s">
-        <v>141</v>
       </c>
       <c r="F126" s="51">
         <v>13993</v>

</xml_diff>